<commit_message>
Changes in PC datasets
</commit_message>
<xml_diff>
--- a/Data/Pregnancy_Complications_Datasets.xlsx
+++ b/Data/Pregnancy_Complications_Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marta/Desktop/Universitat/3_ANY/TFG/TFG_GitHub/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marta/Documents/GitHub/FGP_Marta_Ibanez/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DC85DD-C92E-A64D-9280-1B2B2A2BC296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6571D551-8C37-CF4B-9A22-4F337B68E75A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="27480" windowHeight="16020" xr2:uid="{20F47280-C398-9347-BB38-0902E2B8B33C}"/>
+    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{20F47280-C398-9347-BB38-0902E2B8B33C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>Complications</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">GSM635904-GSM635926 </t>
   </si>
   <si>
-    <t xml:space="preserve">N=23 (microarray) </t>
-  </si>
-  <si>
     <t xml:space="preserve">GSE4707: </t>
   </si>
   <si>
@@ -120,9 +117,6 @@
   </si>
   <si>
     <t xml:space="preserve">GSE35574: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N=19 (microarray) </t>
   </si>
   <si>
     <t>GSM871047,49,50,70,76,80,81,91,94,96,
@@ -232,24 +226,35 @@
 cytotrophoblasts) </t>
   </si>
   <si>
-    <t xml:space="preserve">N=17 (Severe
- Preeclampsia) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N=8 (Severe 
-Preeclampsia) </t>
-  </si>
-  <si>
     <t xml:space="preserve">N=8 (Chorionic Villi,
  Early-Onset Preeclampsia) </t>
   </si>
   <si>
-    <t>N=6 Preeclampsia
- Placental Tissue</t>
-  </si>
-  <si>
     <t xml:space="preserve">N=4 (6 week, 2 replicates,
  8 week, 14.6 week) </t>
+  </si>
+  <si>
+    <t>N=6 PE
+ Placental Tissue</t>
+  </si>
+  <si>
+    <t>N=23 , PE placenta, 
+(microarray)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=19, PE, placenta, 
+(microarray) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=8 (Severe 
+PE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N=17 (Severe
+ PE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSM2463686-GSM2463688 </t>
   </si>
 </sst>
 </file>
@@ -281,7 +286,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -372,11 +377,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -405,9 +423,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -426,6 +441,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7366403-062F-EB49-90EC-D1DF3E5B3F80}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,7 +805,7 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -786,17 +814,17 @@
         <v>6</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="13"/>
     </row>
@@ -806,324 +834,324 @@
         <v>7</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="13"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="13" t="s">
-        <v>59</v>
+      <c r="C6" s="19"/>
+      <c r="D6" s="25" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="13"/>
+      <c r="C7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="13" t="s">
-        <v>58</v>
+      <c r="C8" s="19"/>
+      <c r="D8" s="25" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="13"/>
+      <c r="C9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="13"/>
+      <c r="C11" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="26"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="13"/>
+      <c r="C15" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="13"/>
+      <c r="C17" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="20"/>
+        <v>27</v>
+      </c>
+      <c r="C21" s="9"/>
       <c r="D21" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="13"/>
+      <c r="B22" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="2" t="s">
-        <v>53</v>
+      <c r="B25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="28" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="2" t="s">
-        <v>52</v>
+      <c r="B26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="28" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>50</v>
+      <c r="B30" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="26" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>47</v>
+      <c r="B34" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>